<commit_message>
ACTUALIZACIÓN DE SOFTWARE PRE-FINAL
</commit_message>
<xml_diff>
--- a/Detalles/Planificacion/Planificacion.xlsx
+++ b/Detalles/Planificacion/Planificacion.xlsx
@@ -161,12 +161,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,34 +464,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -562,7 +562,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -577,7 +577,7 @@
       <c r="E8" s="2">
         <v>43868</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="4">
         <v>1</v>
       </c>
@@ -593,7 +593,7 @@
       <c r="E9" s="2">
         <v>43870</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="4">
         <v>0</v>
       </c>
@@ -609,7 +609,7 @@
       <c r="E10" s="2">
         <v>43875</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="4">
         <v>0</v>
       </c>
@@ -621,7 +621,7 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -636,7 +636,7 @@
       <c r="E12" s="2">
         <v>43868</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="4">
         <v>1</v>
       </c>
@@ -652,7 +652,7 @@
       <c r="E13" s="2">
         <v>43870</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="4">
         <v>1</v>
       </c>
@@ -668,7 +668,7 @@
       <c r="E14" s="2">
         <v>43875</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="4">
         <v>0</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="E15" s="2">
         <v>43868</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -701,7 +701,7 @@
       <c r="E16" s="2">
         <v>43868</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="4">
         <v>1</v>
       </c>
@@ -718,7 +718,7 @@
       <c r="E17" s="2">
         <v>43870</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="4">
         <v>0</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="E18" s="2">
         <v>43875</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="4">
         <v>0</v>
       </c>
@@ -752,7 +752,7 @@
       <c r="E19" s="2">
         <v>43868</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -767,7 +767,7 @@
       <c r="E20" s="2">
         <v>43868</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="4">
         <v>1</v>
       </c>
@@ -783,7 +783,7 @@
       <c r="E21" s="2">
         <v>43870</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="4">
         <v>1</v>
       </c>
@@ -799,9 +799,9 @@
       <c r="E22" s="2">
         <v>43875</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
       <c r="E23" s="2">
         <v>43868</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -832,7 +832,7 @@
       <c r="E24" s="2">
         <v>43868</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="4">
         <v>1</v>
       </c>
@@ -848,7 +848,7 @@
       <c r="E25" s="2">
         <v>43870</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="4">
         <v>0</v>
       </c>
@@ -864,7 +864,7 @@
       <c r="E26" s="2">
         <v>43875</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="4">
         <v>0</v>
       </c>
@@ -911,16 +911,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F15:F18"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F15:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>